<commit_message>
This is been Changed miskekenly
</commit_message>
<xml_diff>
--- a/myexcelrenamed.xlsx
+++ b/myexcelrenamed.xlsx
@@ -14,27 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">Name </t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>Satish Dipke</t>
-  </si>
-  <si>
-    <t>Manisha</t>
-  </si>
-  <si>
-    <t>swapnil</t>
+    <t xml:space="preserve">jj knb </t>
   </si>
 </sst>
 </file>
@@ -376,68 +358,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E5"/>
+  <dimension ref="A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>40</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>40</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>40</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>